<commit_message>
PSNUxIM - KP_PREV keypop update PREP_CURR to PREP_ct, update ages 65+
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D842367B-2F33-094D-A2F6-894CF9EF34C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5AA7E655-0270-3A45-8363-671ACD454B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40080" yWindow="1100" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37720" yWindow="1100" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1624" uniqueCount="431">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1624" uniqueCount="433">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -704,9 +704,6 @@
     <t>tr_pos</t>
   </si>
   <si>
-    <t>kp2</t>
-  </si>
-  <si>
     <t>&lt;1-18+</t>
   </si>
   <si>
@@ -725,9 +722,6 @@
     <t>tss_NewPos</t>
   </si>
   <si>
-    <t>&lt;1-50+</t>
-  </si>
-  <si>
     <t>&lt;15, Female, Routine, Positive</t>
   </si>
   <si>
@@ -1139,12 +1133,6 @@
     <t>PP_PREV.T</t>
   </si>
   <si>
-    <t>PrEP_CURR.T</t>
-  </si>
-  <si>
-    <t>PrEP_CURR.KP.T</t>
-  </si>
-  <si>
     <t>PrEP_NEW.T</t>
   </si>
   <si>
@@ -1332,6 +1320,24 @@
   </si>
   <si>
     <t>2021Oct</t>
+  </si>
+  <si>
+    <t>PrEP_CT.T</t>
+  </si>
+  <si>
+    <t>PrEP_CT.KP.T</t>
+  </si>
+  <si>
+    <t>1-65+</t>
+  </si>
+  <si>
+    <t>10-65+</t>
+  </si>
+  <si>
+    <t>&lt;1-65+</t>
+  </si>
+  <si>
+    <t>15-65+</t>
   </si>
 </sst>
 </file>
@@ -1492,7 +1498,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1675,6 +1681,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1865,7 +1877,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1878,6 +1890,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="6" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="10" xfId="6" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2244,23 +2259,23 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="topRight" activeCell="J89" sqref="J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -2271,31 +2286,31 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>287</v>
+        <v>305</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>285</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>78</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>288</v>
+        <v>241</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>286</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>80</v>
@@ -2307,7 +2322,7 @@
         <v>82</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>88</v>
@@ -2315,31 +2330,31 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>429</v>
+        <v>310</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>430</v>
+        <v>283</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>
@@ -2359,31 +2374,31 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>429</v>
+        <v>311</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>430</v>
+        <v>283</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>9</v>
@@ -2403,34 +2418,34 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>429</v>
+        <v>312</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>86</v>
+        <v>270</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>429</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>85</v>
@@ -2439,7 +2454,7 @@
         <v>9</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>89</v>
@@ -2447,34 +2462,34 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>429</v>
+        <v>313</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>86</v>
+        <v>270</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>429</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>85</v>
@@ -2483,7 +2498,7 @@
         <v>9</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>89</v>
@@ -2491,31 +2506,31 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>429</v>
+        <v>314</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>430</v>
+        <v>411</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>95</v>
@@ -2535,34 +2550,34 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>429</v>
+        <v>315</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>58</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>86</v>
+        <v>269</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>429</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>85</v>
@@ -2571,7 +2586,7 @@
         <v>9</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>89</v>
@@ -2579,34 +2594,34 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>429</v>
+        <v>316</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>58</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>86</v>
+        <v>269</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>429</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>85</v>
@@ -2615,7 +2630,7 @@
         <v>9</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>89</v>
@@ -2623,31 +2638,31 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>429</v>
+        <v>317</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>430</v>
+        <v>412</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>95</v>
@@ -2667,31 +2682,31 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>429</v>
+        <v>318</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>430</v>
+        <v>265</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>84</v>
@@ -2711,31 +2726,31 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>429</v>
+        <v>319</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>61</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>430</v>
+        <v>268</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>86</v>
@@ -2755,31 +2770,31 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>429</v>
+        <v>320</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>61</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>430</v>
+        <v>268</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>86</v>
@@ -2799,31 +2814,31 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>429</v>
+        <v>321</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>430</v>
+        <v>413</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>95</v>
@@ -2843,31 +2858,31 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>429</v>
+        <v>322</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>430</v>
+        <v>271</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>86</v>
@@ -2887,31 +2902,31 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>429</v>
+        <v>323</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>430</v>
+        <v>271</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>86</v>
@@ -2931,31 +2946,31 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>429</v>
+        <v>324</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>430</v>
+        <v>414</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>95</v>
@@ -2975,31 +2990,31 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>429</v>
+        <v>325</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>430</v>
+        <v>275</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>87</v>
@@ -3019,31 +3034,31 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>429</v>
+        <v>326</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>430</v>
+        <v>275</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>87</v>
@@ -3063,31 +3078,31 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>429</v>
+        <v>327</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>53</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>430</v>
+        <v>284</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>86</v>
@@ -3107,31 +3122,31 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>429</v>
+        <v>328</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>53</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>430</v>
+        <v>284</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>86</v>
@@ -3151,31 +3166,31 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>429</v>
+        <v>329</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>430</v>
+        <v>415</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>95</v>
@@ -3195,31 +3210,31 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>429</v>
+        <v>330</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>68</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>430</v>
+        <v>277</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>86</v>
@@ -3239,31 +3254,31 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>429</v>
+        <v>331</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>68</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>430</v>
+        <v>277</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>86</v>
@@ -3283,31 +3298,31 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>429</v>
+        <v>332</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>430</v>
+        <v>416</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>95</v>
@@ -3327,31 +3342,31 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>429</v>
+        <v>333</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>55</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>430</v>
+        <v>278</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>86</v>
@@ -3371,31 +3386,31 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>429</v>
+        <v>334</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>55</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>430</v>
+        <v>278</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>86</v>
@@ -3415,31 +3430,31 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>429</v>
+        <v>335</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>430</v>
+        <v>417</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>95</v>
@@ -3459,31 +3474,31 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>429</v>
+        <v>336</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>430</v>
+        <v>279</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>87</v>
@@ -3503,31 +3518,31 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>429</v>
+        <v>337</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>430</v>
+        <v>279</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>87</v>
@@ -3547,34 +3562,34 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>429</v>
+        <v>338</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="I30" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J30" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>94</v>
@@ -3591,34 +3606,34 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>429</v>
+        <v>339</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="I31" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J31" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>94</v>
@@ -3635,31 +3650,31 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>429</v>
+        <v>340</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>430</v>
+        <v>418</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>95</v>
@@ -3679,31 +3694,31 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>429</v>
+        <v>341</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>63</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>430</v>
+        <v>281</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>86</v>
@@ -3723,31 +3738,31 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>429</v>
+        <v>342</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>63</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>430</v>
+        <v>281</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>86</v>
@@ -3767,31 +3782,31 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>429</v>
+        <v>343</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>430</v>
+        <v>419</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>95</v>
@@ -3811,31 +3826,31 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>429</v>
+        <v>344</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>430</v>
+        <v>282</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>86</v>
@@ -3855,31 +3870,31 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>429</v>
+        <v>345</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>430</v>
+        <v>282</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>86</v>
@@ -3899,31 +3914,31 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>429</v>
+        <v>346</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>430</v>
+        <v>420</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>95</v>
@@ -3943,31 +3958,31 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>429</v>
+        <v>347</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>430</v>
+        <v>274</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J39" s="6" t="s">
         <v>9</v>
@@ -3987,31 +4002,31 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>429</v>
+        <v>348</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>430</v>
+        <v>274</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>9</v>
@@ -4031,31 +4046,31 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>429</v>
+        <v>349</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>430</v>
+        <v>272</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>9</v>
@@ -4075,31 +4090,31 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>429</v>
+        <v>350</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>430</v>
+        <v>273</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>9</v>
@@ -4119,31 +4134,31 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>429</v>
+        <v>351</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>430</v>
+        <v>280</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>9</v>
@@ -4163,31 +4178,31 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>429</v>
+        <v>352</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>430</v>
+        <v>272</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>9</v>
@@ -4195,8 +4210,8 @@
       <c r="K44" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L44" s="6" t="s">
-        <v>221</v>
+      <c r="L44" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="M44" s="4" t="s">
         <v>9</v>
@@ -4207,31 +4222,31 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>429</v>
+        <v>353</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>430</v>
+        <v>276</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>9</v>
@@ -4251,34 +4266,34 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>429</v>
+        <v>354</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>430</v>
+        <v>309</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K46" s="6" t="s">
         <v>85</v>
@@ -4287,7 +4302,7 @@
         <v>9</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>89</v>
@@ -4295,34 +4310,34 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>428</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>429</v>
+        <v>424</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>430</v>
+        <v>309</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J47" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K47" s="6" t="s">
         <v>85</v>
@@ -4331,7 +4346,7 @@
         <v>9</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>89</v>
@@ -4339,34 +4354,34 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>429</v>
+        <v>421</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>430</v>
+        <v>309</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="K48" s="6" t="s">
         <v>85</v>
@@ -4375,7 +4390,7 @@
         <v>9</v>
       </c>
       <c r="M48" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>89</v>
@@ -4383,34 +4398,34 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>429</v>
+        <v>355</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="I49" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J49" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="K49" s="6" t="s">
         <v>94</v>
@@ -4419,7 +4434,7 @@
         <v>9</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>89</v>
@@ -4427,34 +4442,34 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>429</v>
+        <v>356</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="I50" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J50" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="K50" s="6" t="s">
         <v>94</v>
@@ -4463,7 +4478,7 @@
         <v>9</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>89</v>
@@ -4471,31 +4486,31 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>429</v>
+        <v>357</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>29</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>430</v>
+        <v>264</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>92</v>
@@ -4515,31 +4530,31 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>429</v>
+        <v>358</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>29</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>430</v>
+        <v>264</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>93</v>
@@ -4559,34 +4574,34 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>429</v>
+        <v>359</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="I53" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J53" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>94</v>
@@ -4603,34 +4618,34 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>429</v>
+        <v>360</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I54" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J54" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="J54" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="K54" s="6" t="s">
         <v>94</v>
@@ -4639,7 +4654,7 @@
         <v>9</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>89</v>
@@ -4647,34 +4662,34 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>429</v>
+        <v>361</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I55" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J55" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>94</v>
@@ -4683,7 +4698,7 @@
         <v>9</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>89</v>
@@ -4691,34 +4706,34 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>429</v>
+        <v>362</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I56" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J56" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="K56" s="6" t="s">
         <v>94</v>
@@ -4727,7 +4742,7 @@
         <v>9</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>89</v>
@@ -4735,31 +4750,31 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>429</v>
+        <v>423</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>430</v>
+        <v>396</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>95</v>
@@ -4779,31 +4794,31 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>429</v>
+        <v>363</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>430</v>
+        <v>265</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>84</v>
@@ -4822,32 +4837,32 @@
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>429</v>
+      <c r="A59" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>430</v>
+        <v>265</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>95</v>
@@ -4866,32 +4881,32 @@
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>429</v>
+      <c r="A60" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>430</v>
+        <v>272</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J60" s="6" t="s">
         <v>9</v>
@@ -4911,31 +4926,31 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>429</v>
+        <v>364</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>430</v>
+        <v>265</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>95</v>
@@ -4955,31 +4970,31 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>429</v>
+        <v>365</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>430</v>
+        <v>272</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>9</v>
@@ -4999,34 +5014,34 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>429</v>
+        <v>366</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>228</v>
+        <v>293</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J63" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K63" s="6" t="s">
         <v>85</v>
@@ -5035,7 +5050,7 @@
         <v>9</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>89</v>
@@ -5043,34 +5058,34 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>429</v>
+        <v>367</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>228</v>
+        <v>293</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J64" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K64" s="6" t="s">
         <v>85</v>
@@ -5079,7 +5094,7 @@
         <v>9</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>89</v>
@@ -5087,34 +5102,34 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>429</v>
+        <v>368</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>430</v>
+        <v>293</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K65" s="6" t="s">
         <v>85</v>
@@ -5123,7 +5138,7 @@
         <v>9</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N65" s="4" t="s">
         <v>89</v>
@@ -5131,34 +5146,34 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>429</v>
+        <v>369</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="I66" s="4" t="s">
-        <v>430</v>
+        <v>293</v>
+      </c>
+      <c r="I66" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K66" s="6" t="s">
         <v>85</v>
@@ -5167,7 +5182,7 @@
         <v>9</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N66" s="4" t="s">
         <v>89</v>
@@ -5175,34 +5190,34 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>429</v>
+        <v>370</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="I67" s="4" t="s">
-        <v>430</v>
+        <v>293</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K67" s="6" t="s">
         <v>85</v>
@@ -5211,7 +5226,7 @@
         <v>9</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>89</v>
@@ -5219,34 +5234,34 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>429</v>
+        <v>371</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>430</v>
+        <v>293</v>
+      </c>
+      <c r="I68" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K68" s="6" t="s">
         <v>85</v>
@@ -5255,7 +5270,7 @@
         <v>9</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N68" s="4" t="s">
         <v>89</v>
@@ -5263,34 +5278,34 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>429</v>
+        <v>372</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="I69" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J69" s="4" t="s">
-        <v>228</v>
+        <v>265</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J69" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K69" s="6" t="s">
         <v>85</v>
@@ -5307,34 +5322,34 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>429</v>
+        <v>373</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I70" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>228</v>
+        <v>267</v>
+      </c>
+      <c r="I70" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J70" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K70" s="6" t="s">
         <v>85</v>
@@ -5343,7 +5358,7 @@
         <v>9</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N70" s="4" t="s">
         <v>89</v>
@@ -5351,34 +5366,34 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>429</v>
+        <v>374</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I71" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J71" s="4" t="s">
-        <v>228</v>
+        <v>267</v>
+      </c>
+      <c r="I71" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J71" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K71" s="6" t="s">
         <v>85</v>
@@ -5387,7 +5402,7 @@
         <v>9</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N71" s="4" t="s">
         <v>89</v>
@@ -5395,34 +5410,34 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>429</v>
+        <v>375</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="I72" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>228</v>
+        <v>267</v>
+      </c>
+      <c r="I72" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J72" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K72" s="6" t="s">
         <v>85</v>
@@ -5431,7 +5446,7 @@
         <v>9</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N72" s="4" t="s">
         <v>89</v>
@@ -5439,31 +5454,31 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>429</v>
+        <v>376</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="H73" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="I73" s="4" t="s">
-        <v>430</v>
+      <c r="I73" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>95</v>
@@ -5483,34 +5498,34 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>429</v>
+        <v>377</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="I74" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J74" s="4" t="s">
-        <v>228</v>
+        <v>266</v>
+      </c>
+      <c r="I74" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J74" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K74" s="6" t="s">
         <v>85</v>
@@ -5527,34 +5542,34 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>429</v>
+        <v>378</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>228</v>
+        <v>266</v>
+      </c>
+      <c r="I75" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J75" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K75" s="6" t="s">
         <v>85</v>
@@ -5571,31 +5586,31 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>429</v>
+        <v>379</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>430</v>
+        <v>273</v>
+      </c>
+      <c r="I76" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J76" s="6" t="s">
         <v>9</v>
@@ -5615,31 +5630,31 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>429</v>
+        <v>380</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I77" s="4" t="s">
-        <v>430</v>
+        <v>273</v>
+      </c>
+      <c r="I77" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>9</v>
@@ -5659,31 +5674,31 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>429</v>
+        <v>381</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I78" s="4" t="s">
-        <v>430</v>
+        <v>273</v>
+      </c>
+      <c r="I78" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J78" s="6" t="s">
         <v>9</v>
@@ -5703,31 +5718,31 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>429</v>
+        <v>382</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="I79" s="4" t="s">
-        <v>430</v>
+        <v>273</v>
+      </c>
+      <c r="I79" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J79" s="6" t="s">
         <v>9</v>
@@ -5747,34 +5762,34 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>429</v>
+        <v>383</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>228</v>
+        <v>295</v>
+      </c>
+      <c r="I80" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J80" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K80" s="6" t="s">
         <v>85</v>
@@ -5783,7 +5798,7 @@
         <v>9</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N80" s="4" t="s">
         <v>89</v>
@@ -5791,34 +5806,34 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>429</v>
+        <v>384</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="I81" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>228</v>
+        <v>295</v>
+      </c>
+      <c r="I81" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J81" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="K81" s="6" t="s">
         <v>85</v>
@@ -5827,7 +5842,7 @@
         <v>9</v>
       </c>
       <c r="M81" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N81" s="4" t="s">
         <v>89</v>
@@ -5835,34 +5850,34 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>429</v>
+        <v>385</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="I82" s="4" t="s">
-        <v>430</v>
+        <v>299</v>
+      </c>
+      <c r="I82" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K82" s="6" t="s">
         <v>85</v>
@@ -5871,7 +5886,7 @@
         <v>9</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N82" s="4" t="s">
         <v>89</v>
@@ -5879,34 +5894,34 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>429</v>
+        <v>386</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="I83" s="4" t="s">
-        <v>430</v>
+        <v>299</v>
+      </c>
+      <c r="I83" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K83" s="6" t="s">
         <v>85</v>
@@ -5915,7 +5930,7 @@
         <v>9</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N83" s="4" t="s">
         <v>89</v>
@@ -5923,34 +5938,34 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>429</v>
+        <v>387</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="I84" s="4" t="s">
-        <v>430</v>
+        <v>299</v>
+      </c>
+      <c r="I84" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K84" s="6" t="s">
         <v>85</v>
@@ -5959,7 +5974,7 @@
         <v>9</v>
       </c>
       <c r="M84" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>89</v>
@@ -5967,34 +5982,34 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>429</v>
+        <v>388</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="I85" s="4" t="s">
-        <v>430</v>
+        <v>299</v>
+      </c>
+      <c r="I85" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K85" s="6" t="s">
         <v>85</v>
@@ -6003,7 +6018,7 @@
         <v>9</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="N85" s="4" t="s">
         <v>89</v>
@@ -6011,43 +6026,43 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>429</v>
+        <v>389</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="I86" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>95</v>
+        <v>266</v>
+      </c>
+      <c r="I86" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J86" s="12" t="s">
+        <v>432</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L86" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>89</v>
@@ -6055,43 +6070,43 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>429</v>
+        <v>390</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="I87" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>95</v>
+        <v>266</v>
+      </c>
+      <c r="I87" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J87" s="12" t="s">
+        <v>432</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L87" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>89</v>
@@ -6099,37 +6114,37 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>429</v>
+        <v>391</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="I88" s="4" t="s">
-        <v>430</v>
+        <v>400</v>
+      </c>
+      <c r="I88" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>95</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L88" s="6" t="s">
         <v>9</v>
@@ -6143,43 +6158,43 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>429</v>
+        <v>392</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="I89" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>95</v>
+        <v>266</v>
+      </c>
+      <c r="I89" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="J89" s="12" t="s">
+        <v>432</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L89" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M89" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="N89" s="4" t="s">
         <v>89</v>
@@ -6187,31 +6202,31 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>429</v>
+        <v>393</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="I90" s="4" t="s">
-        <v>430</v>
+        <v>266</v>
+      </c>
+      <c r="I90" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>95</v>
@@ -7018,49 +7033,49 @@
     <row r="73" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E73" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G73" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E74" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G74" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E75" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G75" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E76" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G76" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PSNUxIM distribution Update OVC_SERV indicators
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5AA7E655-0270-3A45-8363-671ACD454B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9588992D-F5FE-864D-8540-5382078B2616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37720" yWindow="1100" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1624" uniqueCount="433">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1638" uniqueCount="439">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1338,6 +1338,24 @@
   </si>
   <si>
     <t>15-65+</t>
+  </si>
+  <si>
+    <t>OVC_SERV.DREAMS.T</t>
+  </si>
+  <si>
+    <t>DE_GROUP-bEEWV7SqvjQ</t>
+  </si>
+  <si>
+    <t>wqHjTjIvhlw</t>
+  </si>
+  <si>
+    <t>Age/Sex/Preventive</t>
+  </si>
+  <si>
+    <t>cCTvqWoHxSk</t>
+  </si>
+  <si>
+    <t>Age/Sex/DREAMS</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1516,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1690,6 +1708,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1877,7 +1901,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1888,11 +1912,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="6" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="10" xfId="6" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="10" xfId="7" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="35" borderId="10" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="8" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2257,25 +2287,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N90"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="J89" sqref="J89"/>
+      <selection pane="topRight" activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -2288,7 +2318,7 @@
       <c r="A1" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -2309,7 +2339,7 @@
       <c r="H1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>286</v>
       </c>
       <c r="J1" s="4" t="s">
@@ -2332,7 +2362,7 @@
       <c r="A2" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -2353,7 +2383,7 @@
       <c r="H2" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -2376,7 +2406,7 @@
       <c r="A3" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2397,7 +2427,7 @@
       <c r="H3" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -2420,7 +2450,7 @@
       <c r="A4" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2441,10 +2471,10 @@
       <c r="H4" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J4" s="12" t="s">
+      <c r="I4" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>429</v>
       </c>
       <c r="K4" s="6" t="s">
@@ -2464,7 +2494,7 @@
       <c r="A5" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -2485,10 +2515,10 @@
       <c r="H5" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J5" s="12" t="s">
+      <c r="I5" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>429</v>
       </c>
       <c r="K5" s="6" t="s">
@@ -2508,7 +2538,7 @@
       <c r="A6" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -2529,7 +2559,7 @@
       <c r="H6" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -2552,7 +2582,7 @@
       <c r="A7" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -2573,10 +2603,10 @@
       <c r="H7" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J7" s="12" t="s">
+      <c r="I7" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>429</v>
       </c>
       <c r="K7" s="6" t="s">
@@ -2596,7 +2626,7 @@
       <c r="A8" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -2617,10 +2647,10 @@
       <c r="H8" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J8" s="12" t="s">
+      <c r="I8" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>429</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -2640,7 +2670,7 @@
       <c r="A9" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -2661,7 +2691,7 @@
       <c r="H9" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J9" s="4" t="s">
@@ -2684,7 +2714,7 @@
       <c r="A10" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -2705,7 +2735,7 @@
       <c r="H10" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -2728,7 +2758,7 @@
       <c r="A11" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2749,7 +2779,7 @@
       <c r="H11" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J11" s="4" t="s">
@@ -2772,7 +2802,7 @@
       <c r="A12" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -2793,7 +2823,7 @@
       <c r="H12" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J12" s="4" t="s">
@@ -2816,7 +2846,7 @@
       <c r="A13" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2837,7 +2867,7 @@
       <c r="H13" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -2860,7 +2890,7 @@
       <c r="A14" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -2881,7 +2911,7 @@
       <c r="H14" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J14" s="4" t="s">
@@ -2904,7 +2934,7 @@
       <c r="A15" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -2925,7 +2955,7 @@
       <c r="H15" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J15" s="4" t="s">
@@ -2948,7 +2978,7 @@
       <c r="A16" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -2969,7 +2999,7 @@
       <c r="H16" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J16" s="4" t="s">
@@ -2992,7 +3022,7 @@
       <c r="A17" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -3013,7 +3043,7 @@
       <c r="H17" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J17" s="4" t="s">
@@ -3036,7 +3066,7 @@
       <c r="A18" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -3057,7 +3087,7 @@
       <c r="H18" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J18" s="4" t="s">
@@ -3080,7 +3110,7 @@
       <c r="A19" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -3101,7 +3131,7 @@
       <c r="H19" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J19" s="4" t="s">
@@ -3124,7 +3154,7 @@
       <c r="A20" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -3145,7 +3175,7 @@
       <c r="H20" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J20" s="4" t="s">
@@ -3168,7 +3198,7 @@
       <c r="A21" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -3189,7 +3219,7 @@
       <c r="H21" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I21" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J21" s="4" t="s">
@@ -3212,7 +3242,7 @@
       <c r="A22" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -3233,7 +3263,7 @@
       <c r="H22" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="I22" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J22" s="4" t="s">
@@ -3256,7 +3286,7 @@
       <c r="A23" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -3277,7 +3307,7 @@
       <c r="H23" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="I23" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J23" s="4" t="s">
@@ -3300,7 +3330,7 @@
       <c r="A24" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -3321,7 +3351,7 @@
       <c r="H24" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I24" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J24" s="4" t="s">
@@ -3344,7 +3374,7 @@
       <c r="A25" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -3365,7 +3395,7 @@
       <c r="H25" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="I25" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -3388,7 +3418,7 @@
       <c r="A26" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -3409,7 +3439,7 @@
       <c r="H26" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="I26" s="12" t="s">
+      <c r="I26" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J26" s="4" t="s">
@@ -3432,7 +3462,7 @@
       <c r="A27" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -3453,7 +3483,7 @@
       <c r="H27" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="I27" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J27" s="4" t="s">
@@ -3476,7 +3506,7 @@
       <c r="A28" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -3497,7 +3527,7 @@
       <c r="H28" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J28" s="4" t="s">
@@ -3520,7 +3550,7 @@
       <c r="A29" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -3541,7 +3571,7 @@
       <c r="H29" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J29" s="4" t="s">
@@ -3564,7 +3594,7 @@
       <c r="A30" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -3585,10 +3615,10 @@
       <c r="H30" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="I30" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J30" s="12" t="s">
+      <c r="I30" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J30" s="11" t="s">
         <v>430</v>
       </c>
       <c r="K30" s="6" t="s">
@@ -3608,7 +3638,7 @@
       <c r="A31" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -3629,10 +3659,10 @@
       <c r="H31" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J31" s="12" t="s">
+      <c r="I31" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J31" s="11" t="s">
         <v>430</v>
       </c>
       <c r="K31" s="6" t="s">
@@ -3652,7 +3682,7 @@
       <c r="A32" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -3673,7 +3703,7 @@
       <c r="H32" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I32" s="12" t="s">
+      <c r="I32" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J32" s="4" t="s">
@@ -3696,7 +3726,7 @@
       <c r="A33" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -3717,7 +3747,7 @@
       <c r="H33" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="I33" s="12" t="s">
+      <c r="I33" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J33" s="4" t="s">
@@ -3740,7 +3770,7 @@
       <c r="A34" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -3761,7 +3791,7 @@
       <c r="H34" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="I34" s="12" t="s">
+      <c r="I34" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J34" s="4" t="s">
@@ -3784,7 +3814,7 @@
       <c r="A35" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -3805,7 +3835,7 @@
       <c r="H35" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="I35" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J35" s="4" t="s">
@@ -3828,7 +3858,7 @@
       <c r="A36" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -3849,7 +3879,7 @@
       <c r="H36" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="I36" s="12" t="s">
+      <c r="I36" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J36" s="4" t="s">
@@ -3872,7 +3902,7 @@
       <c r="A37" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -3893,7 +3923,7 @@
       <c r="H37" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="I37" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J37" s="4" t="s">
@@ -3916,7 +3946,7 @@
       <c r="A38" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -3937,7 +3967,7 @@
       <c r="H38" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="I38" s="12" t="s">
+      <c r="I38" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J38" s="4" t="s">
@@ -3960,7 +3990,7 @@
       <c r="A39" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -3981,7 +4011,7 @@
       <c r="H39" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="I39" s="12" t="s">
+      <c r="I39" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J39" s="6" t="s">
@@ -4004,7 +4034,7 @@
       <c r="A40" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -4025,7 +4055,7 @@
       <c r="H40" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="I40" s="12" t="s">
+      <c r="I40" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J40" s="6" t="s">
@@ -4048,7 +4078,7 @@
       <c r="A41" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -4069,7 +4099,7 @@
       <c r="H41" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="I41" s="12" t="s">
+      <c r="I41" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J41" s="6" t="s">
@@ -4092,7 +4122,7 @@
       <c r="A42" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -4113,7 +4143,7 @@
       <c r="H42" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="I42" s="12" t="s">
+      <c r="I42" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J42" s="6" t="s">
@@ -4136,7 +4166,7 @@
       <c r="A43" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -4157,7 +4187,7 @@
       <c r="H43" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="I43" s="12" t="s">
+      <c r="I43" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J43" s="4" t="s">
@@ -4180,7 +4210,7 @@
       <c r="A44" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -4201,7 +4231,7 @@
       <c r="H44" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="I44" s="12" t="s">
+      <c r="I44" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J44" s="6" t="s">
@@ -4210,7 +4240,7 @@
       <c r="K44" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L44" s="14" t="s">
+      <c r="L44" s="13" t="s">
         <v>90</v>
       </c>
       <c r="M44" s="4" t="s">
@@ -4224,7 +4254,7 @@
       <c r="A45" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -4245,7 +4275,7 @@
       <c r="H45" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="I45" s="12" t="s">
+      <c r="I45" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J45" s="4" t="s">
@@ -4268,7 +4298,7 @@
       <c r="A46" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C46" s="8" t="s">
@@ -4289,7 +4319,7 @@
       <c r="H46" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="I46" s="12" t="s">
+      <c r="I46" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J46" s="8" t="s">
@@ -4312,7 +4342,7 @@
       <c r="A47" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -4333,7 +4363,7 @@
       <c r="H47" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="I47" s="12" t="s">
+      <c r="I47" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J47" s="8" t="s">
@@ -4353,46 +4383,46 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="B48" s="12" t="s">
-        <v>425</v>
-      </c>
-      <c r="C48" s="8" t="s">
+      <c r="B48" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C48" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E48" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="I48" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J48" s="10" t="s">
+      <c r="E48" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="J48" s="17" t="s">
         <v>422</v>
       </c>
-      <c r="K48" s="6" t="s">
+      <c r="K48" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="L48" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M48" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="N48" s="4" t="s">
+      <c r="L48" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N48" s="14" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4400,7 +4430,7 @@
       <c r="A49" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -4421,10 +4451,10 @@
       <c r="H49" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="I49" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J49" s="12" t="s">
+      <c r="I49" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J49" s="11" t="s">
         <v>430</v>
       </c>
       <c r="K49" s="6" t="s">
@@ -4444,7 +4474,7 @@
       <c r="A50" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -4465,10 +4495,10 @@
       <c r="H50" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="I50" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J50" s="12" t="s">
+      <c r="I50" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J50" s="11" t="s">
         <v>430</v>
       </c>
       <c r="K50" s="6" t="s">
@@ -4488,7 +4518,7 @@
       <c r="A51" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -4509,7 +4539,7 @@
       <c r="H51" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="I51" s="12" t="s">
+      <c r="I51" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J51" s="4" t="s">
@@ -4532,7 +4562,7 @@
       <c r="A52" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -4553,7 +4583,7 @@
       <c r="H52" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="I52" s="12" t="s">
+      <c r="I52" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J52" s="4" t="s">
@@ -4576,7 +4606,7 @@
       <c r="A53" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -4597,10 +4627,10 @@
       <c r="H53" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="I53" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J53" s="12" t="s">
+      <c r="I53" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J53" s="11" t="s">
         <v>430</v>
       </c>
       <c r="K53" s="6" t="s">
@@ -4620,7 +4650,7 @@
       <c r="A54" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -4641,10 +4671,10 @@
       <c r="H54" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="I54" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J54" s="12" t="s">
+      <c r="I54" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J54" s="11" t="s">
         <v>430</v>
       </c>
       <c r="K54" s="6" t="s">
@@ -4664,7 +4694,7 @@
       <c r="A55" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -4685,10 +4715,10 @@
       <c r="H55" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="I55" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J55" s="12" t="s">
+      <c r="I55" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J55" s="11" t="s">
         <v>430</v>
       </c>
       <c r="K55" s="6" t="s">
@@ -4708,7 +4738,7 @@
       <c r="A56" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -4729,10 +4759,10 @@
       <c r="H56" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="I56" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J56" s="12" t="s">
+      <c r="I56" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J56" s="11" t="s">
         <v>430</v>
       </c>
       <c r="K56" s="6" t="s">
@@ -4752,7 +4782,7 @@
       <c r="A57" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -4773,7 +4803,7 @@
       <c r="H57" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="I57" s="12" t="s">
+      <c r="I57" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J57" s="4" t="s">
@@ -4796,7 +4826,7 @@
       <c r="A58" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -4817,7 +4847,7 @@
       <c r="H58" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="I58" s="12" t="s">
+      <c r="I58" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J58" s="4" t="s">
@@ -4837,10 +4867,10 @@
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B59" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -4861,7 +4891,7 @@
       <c r="H59" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="I59" s="12" t="s">
+      <c r="I59" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J59" s="4" t="s">
@@ -4881,10 +4911,10 @@
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="B60" s="12" t="s">
+      <c r="B60" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -4905,7 +4935,7 @@
       <c r="H60" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="I60" s="12" t="s">
+      <c r="I60" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J60" s="6" t="s">
@@ -4928,7 +4958,7 @@
       <c r="A61" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -4949,7 +4979,7 @@
       <c r="H61" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="I61" s="12" t="s">
+      <c r="I61" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J61" s="4" t="s">
@@ -4972,7 +5002,7 @@
       <c r="A62" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C62" s="4" t="s">
@@ -4993,7 +5023,7 @@
       <c r="H62" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="I62" s="12" t="s">
+      <c r="I62" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J62" s="6" t="s">
@@ -5016,7 +5046,7 @@
       <c r="A63" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B63" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C63" s="4" t="s">
@@ -5037,10 +5067,10 @@
       <c r="H63" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I63" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J63" s="12" t="s">
+      <c r="I63" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J63" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K63" s="6" t="s">
@@ -5060,7 +5090,7 @@
       <c r="A64" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="B64" s="12" t="s">
+      <c r="B64" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C64" s="4" t="s">
@@ -5081,10 +5111,10 @@
       <c r="H64" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I64" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J64" s="12" t="s">
+      <c r="I64" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J64" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K64" s="6" t="s">
@@ -5104,7 +5134,7 @@
       <c r="A65" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -5125,7 +5155,7 @@
       <c r="H65" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I65" s="12" t="s">
+      <c r="I65" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J65" s="4" t="s">
@@ -5148,7 +5178,7 @@
       <c r="A66" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -5169,7 +5199,7 @@
       <c r="H66" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I66" s="12" t="s">
+      <c r="I66" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J66" s="4" t="s">
@@ -5192,7 +5222,7 @@
       <c r="A67" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C67" s="4" t="s">
@@ -5213,7 +5243,7 @@
       <c r="H67" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I67" s="12" t="s">
+      <c r="I67" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J67" s="4" t="s">
@@ -5236,7 +5266,7 @@
       <c r="A68" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="B68" s="12" t="s">
+      <c r="B68" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C68" s="4" t="s">
@@ -5257,7 +5287,7 @@
       <c r="H68" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I68" s="12" t="s">
+      <c r="I68" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J68" s="4" t="s">
@@ -5280,7 +5310,7 @@
       <c r="A69" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="B69" s="12" t="s">
+      <c r="B69" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C69" s="4" t="s">
@@ -5301,10 +5331,10 @@
       <c r="H69" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="I69" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J69" s="12" t="s">
+      <c r="I69" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J69" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K69" s="6" t="s">
@@ -5324,7 +5354,7 @@
       <c r="A70" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B70" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C70" s="4" t="s">
@@ -5345,10 +5375,10 @@
       <c r="H70" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="I70" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J70" s="12" t="s">
+      <c r="I70" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J70" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K70" s="6" t="s">
@@ -5368,7 +5398,7 @@
       <c r="A71" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C71" s="4" t="s">
@@ -5389,10 +5419,10 @@
       <c r="H71" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="I71" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J71" s="12" t="s">
+      <c r="I71" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J71" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K71" s="6" t="s">
@@ -5412,7 +5442,7 @@
       <c r="A72" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C72" s="4" t="s">
@@ -5433,10 +5463,10 @@
       <c r="H72" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="I72" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J72" s="12" t="s">
+      <c r="I72" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J72" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K72" s="6" t="s">
@@ -5456,7 +5486,7 @@
       <c r="A73" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C73" s="4" t="s">
@@ -5477,7 +5507,7 @@
       <c r="H73" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="I73" s="12" t="s">
+      <c r="I73" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J73" s="4" t="s">
@@ -5500,7 +5530,7 @@
       <c r="A74" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C74" s="4" t="s">
@@ -5521,10 +5551,10 @@
       <c r="H74" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I74" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J74" s="12" t="s">
+      <c r="I74" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J74" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K74" s="6" t="s">
@@ -5544,7 +5574,7 @@
       <c r="A75" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C75" s="4" t="s">
@@ -5565,10 +5595,10 @@
       <c r="H75" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I75" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J75" s="12" t="s">
+      <c r="I75" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J75" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K75" s="6" t="s">
@@ -5588,7 +5618,7 @@
       <c r="A76" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="B76" s="12" t="s">
+      <c r="B76" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C76" s="4" t="s">
@@ -5609,7 +5639,7 @@
       <c r="H76" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="I76" s="12" t="s">
+      <c r="I76" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J76" s="6" t="s">
@@ -5632,7 +5662,7 @@
       <c r="A77" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="B77" s="12" t="s">
+      <c r="B77" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -5653,7 +5683,7 @@
       <c r="H77" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="I77" s="12" t="s">
+      <c r="I77" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J77" s="6" t="s">
@@ -5676,7 +5706,7 @@
       <c r="A78" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -5697,7 +5727,7 @@
       <c r="H78" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="I78" s="12" t="s">
+      <c r="I78" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J78" s="6" t="s">
@@ -5720,7 +5750,7 @@
       <c r="A79" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="B79" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -5741,7 +5771,7 @@
       <c r="H79" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="I79" s="12" t="s">
+      <c r="I79" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J79" s="6" t="s">
@@ -5764,7 +5794,7 @@
       <c r="A80" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -5785,10 +5815,10 @@
       <c r="H80" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="I80" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J80" s="12" t="s">
+      <c r="I80" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J80" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K80" s="6" t="s">
@@ -5808,7 +5838,7 @@
       <c r="A81" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -5829,10 +5859,10 @@
       <c r="H81" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="I81" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J81" s="12" t="s">
+      <c r="I81" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J81" s="11" t="s">
         <v>431</v>
       </c>
       <c r="K81" s="6" t="s">
@@ -5852,7 +5882,7 @@
       <c r="A82" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C82" s="4" t="s">
@@ -5873,7 +5903,7 @@
       <c r="H82" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="I82" s="12" t="s">
+      <c r="I82" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J82" s="4" t="s">
@@ -5896,7 +5926,7 @@
       <c r="A83" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="B83" s="12" t="s">
+      <c r="B83" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -5917,7 +5947,7 @@
       <c r="H83" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="I83" s="12" t="s">
+      <c r="I83" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J83" s="4" t="s">
@@ -5940,7 +5970,7 @@
       <c r="A84" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="B84" s="12" t="s">
+      <c r="B84" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C84" s="4" t="s">
@@ -5961,7 +5991,7 @@
       <c r="H84" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="I84" s="12" t="s">
+      <c r="I84" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J84" s="4" t="s">
@@ -5984,7 +6014,7 @@
       <c r="A85" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B85" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -6005,7 +6035,7 @@
       <c r="H85" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="I85" s="12" t="s">
+      <c r="I85" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J85" s="4" t="s">
@@ -6028,7 +6058,7 @@
       <c r="A86" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B86" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C86" s="4" t="s">
@@ -6049,10 +6079,10 @@
       <c r="H86" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I86" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J86" s="12" t="s">
+      <c r="I86" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J86" s="11" t="s">
         <v>432</v>
       </c>
       <c r="K86" s="6" t="s">
@@ -6072,7 +6102,7 @@
       <c r="A87" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B87" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C87" s="4" t="s">
@@ -6093,10 +6123,10 @@
       <c r="H87" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I87" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J87" s="12" t="s">
+      <c r="I87" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J87" s="11" t="s">
         <v>432</v>
       </c>
       <c r="K87" s="6" t="s">
@@ -6116,7 +6146,7 @@
       <c r="A88" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B88" s="12" t="s">
+      <c r="B88" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C88" s="4" t="s">
@@ -6137,7 +6167,7 @@
       <c r="H88" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="I88" s="12" t="s">
+      <c r="I88" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J88" s="4" t="s">
@@ -6160,7 +6190,7 @@
       <c r="A89" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C89" s="4" t="s">
@@ -6181,10 +6211,10 @@
       <c r="H89" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I89" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="J89" s="12" t="s">
+      <c r="I89" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J89" s="11" t="s">
         <v>432</v>
       </c>
       <c r="K89" s="6" t="s">
@@ -6204,7 +6234,7 @@
       <c r="A90" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="B90" s="12" t="s">
+      <c r="B90" s="11" t="s">
         <v>425</v>
       </c>
       <c r="C90" s="5" t="s">
@@ -6225,22 +6255,66 @@
       <c r="H90" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I90" s="12" t="s">
+      <c r="I90" s="11" t="s">
         <v>426</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="K90" s="11" t="s">
+      <c r="K90" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="L90" s="11" t="s">
+      <c r="L90" s="10" t="s">
         <v>9</v>
       </c>
       <c r="M90" s="5" t="s">
         <v>9</v>
       </c>
       <c r="N90" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>434</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D91" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E91" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="G91" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="H91" s="18" t="s">
+        <v>437</v>
+      </c>
+      <c r="I91" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="J91" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="K91" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="L91" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M91" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N91" s="20" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update OVC age category in PSNUxIM distribution
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9588992D-F5FE-864D-8540-5382078B2616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1E6A2871-6E84-9249-B036-D34EB012F8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -704,9 +704,6 @@
     <t>tr_pos</t>
   </si>
   <si>
-    <t>&lt;1-18+</t>
-  </si>
-  <si>
     <t>as_already</t>
   </si>
   <si>
@@ -1356,13 +1353,16 @@
   </si>
   <si>
     <t>Age/Sex/DREAMS</t>
+  </si>
+  <si>
+    <t>&lt;01-18+ (OVC &amp; Caregivers)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1513,6 +1513,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1901,7 +1907,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1923,6 +1929,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="8" applyBorder="1"/>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2289,10 +2298,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="E83" sqref="E83"/>
+      <selection pane="topRight" activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2316,31 +2325,31 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>78</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>241</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>80</v>
@@ -2352,7 +2361,7 @@
         <v>82</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>88</v>
@@ -2360,31 +2369,31 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>
@@ -2404,31 +2413,31 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>9</v>
@@ -2448,34 +2457,34 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>289</v>
-      </c>
       <c r="E4" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>85</v>
@@ -2484,7 +2493,7 @@
         <v>9</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>89</v>
@@ -2492,34 +2501,34 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>289</v>
-      </c>
       <c r="E5" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>85</v>
@@ -2528,7 +2537,7 @@
         <v>9</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>89</v>
@@ -2536,31 +2545,31 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>95</v>
@@ -2580,34 +2589,34 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>289</v>
-      </c>
       <c r="E7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>58</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>85</v>
@@ -2616,7 +2625,7 @@
         <v>9</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>89</v>
@@ -2624,34 +2633,34 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>289</v>
-      </c>
       <c r="E8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>58</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>85</v>
@@ -2660,7 +2669,7 @@
         <v>9</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>89</v>
@@ -2668,31 +2677,31 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>95</v>
@@ -2712,31 +2721,31 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>84</v>
@@ -2756,31 +2765,31 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>61</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>86</v>
@@ -2800,31 +2809,31 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>61</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>86</v>
@@ -2844,31 +2853,31 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>95</v>
@@ -2888,31 +2897,31 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>86</v>
@@ -2932,31 +2941,31 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>86</v>
@@ -2976,31 +2985,31 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>95</v>
@@ -3020,31 +3029,31 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>87</v>
@@ -3064,31 +3073,31 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>87</v>
@@ -3108,31 +3117,31 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>53</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>86</v>
@@ -3152,31 +3161,31 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>53</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>86</v>
@@ -3196,31 +3205,31 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>95</v>
@@ -3240,31 +3249,31 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>68</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>86</v>
@@ -3284,31 +3293,31 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>68</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>86</v>
@@ -3328,31 +3337,31 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>95</v>
@@ -3372,31 +3381,31 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>55</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>86</v>
@@ -3416,31 +3425,31 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>55</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>86</v>
@@ -3460,31 +3469,31 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>95</v>
@@ -3504,31 +3513,31 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>87</v>
@@ -3548,31 +3557,31 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>87</v>
@@ -3592,34 +3601,34 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>94</v>
@@ -3636,34 +3645,34 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>94</v>
@@ -3680,31 +3689,31 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>95</v>
@@ -3724,31 +3733,31 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>63</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>86</v>
@@ -3768,31 +3777,31 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>63</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>86</v>
@@ -3812,31 +3821,31 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>95</v>
@@ -3856,31 +3865,31 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>86</v>
@@ -3900,31 +3909,31 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>86</v>
@@ -3944,31 +3953,31 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>95</v>
@@ -3988,31 +3997,31 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J39" s="6" t="s">
         <v>9</v>
@@ -4032,31 +4041,31 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>9</v>
@@ -4076,31 +4085,31 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>9</v>
@@ -4120,31 +4129,31 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>9</v>
@@ -4164,31 +4173,31 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>9</v>
@@ -4208,31 +4217,31 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>9</v>
@@ -4252,31 +4261,31 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>9</v>
@@ -4296,34 +4305,34 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G46" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="H46" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="H46" s="9" t="s">
-        <v>309</v>
-      </c>
       <c r="I46" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>221</v>
+        <v>425</v>
+      </c>
+      <c r="J46" s="21" t="s">
+        <v>438</v>
       </c>
       <c r="K46" s="6" t="s">
         <v>85</v>
@@ -4332,7 +4341,7 @@
         <v>9</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>89</v>
@@ -4340,34 +4349,34 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G47" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="H47" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="H47" s="9" t="s">
-        <v>309</v>
-      </c>
       <c r="I47" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>221</v>
+        <v>425</v>
+      </c>
+      <c r="J47" s="21" t="s">
+        <v>438</v>
       </c>
       <c r="K47" s="6" t="s">
         <v>85</v>
@@ -4376,7 +4385,7 @@
         <v>9</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>89</v>
@@ -4384,34 +4393,34 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>50</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K48" s="14" t="s">
         <v>85</v>
@@ -4428,34 +4437,34 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G49" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H49" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="H49" s="4" t="s">
-        <v>293</v>
-      </c>
       <c r="I49" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K49" s="6" t="s">
         <v>94</v>
@@ -4464,7 +4473,7 @@
         <v>9</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>89</v>
@@ -4472,34 +4481,34 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G50" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H50" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="H50" s="4" t="s">
-        <v>293</v>
-      </c>
       <c r="I50" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K50" s="6" t="s">
         <v>94</v>
@@ -4508,7 +4517,7 @@
         <v>9</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>89</v>
@@ -4516,31 +4525,31 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>29</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>92</v>
@@ -4560,31 +4569,31 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>29</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>93</v>
@@ -4604,34 +4613,34 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>94</v>
@@ -4648,34 +4657,34 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K54" s="6" t="s">
         <v>94</v>
@@ -4684,7 +4693,7 @@
         <v>9</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>89</v>
@@ -4692,34 +4701,34 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>94</v>
@@ -4728,7 +4737,7 @@
         <v>9</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>89</v>
@@ -4736,34 +4745,34 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K56" s="6" t="s">
         <v>94</v>
@@ -4772,7 +4781,7 @@
         <v>9</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>89</v>
@@ -4780,31 +4789,31 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="G57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="H57" s="1" t="s">
-        <v>396</v>
-      </c>
       <c r="I57" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>95</v>
@@ -4824,31 +4833,31 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>84</v>
@@ -4868,31 +4877,31 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>95</v>
@@ -4912,31 +4921,31 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J60" s="6" t="s">
         <v>9</v>
@@ -4956,31 +4965,31 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>95</v>
@@ -5000,31 +5009,31 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>9</v>
@@ -5044,34 +5053,34 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G63" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="I63" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J63" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K63" s="6" t="s">
         <v>85</v>
@@ -5080,7 +5089,7 @@
         <v>9</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>89</v>
@@ -5088,34 +5097,34 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G64" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="I64" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K64" s="6" t="s">
         <v>85</v>
@@ -5124,7 +5133,7 @@
         <v>9</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>89</v>
@@ -5132,34 +5141,34 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G65" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H65" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="H65" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="I65" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K65" s="6" t="s">
         <v>85</v>
@@ -5168,7 +5177,7 @@
         <v>9</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N65" s="4" t="s">
         <v>89</v>
@@ -5176,34 +5185,34 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G66" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H66" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="I66" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K66" s="6" t="s">
         <v>85</v>
@@ -5212,7 +5221,7 @@
         <v>9</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N66" s="4" t="s">
         <v>89</v>
@@ -5220,34 +5229,34 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G67" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H67" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="H67" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="I67" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K67" s="6" t="s">
         <v>85</v>
@@ -5256,7 +5265,7 @@
         <v>9</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>89</v>
@@ -5264,34 +5273,34 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G68" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H68" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="I68" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K68" s="6" t="s">
         <v>85</v>
@@ -5300,7 +5309,7 @@
         <v>9</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N68" s="4" t="s">
         <v>89</v>
@@ -5308,34 +5317,34 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K69" s="6" t="s">
         <v>85</v>
@@ -5352,34 +5361,34 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K70" s="6" t="s">
         <v>85</v>
@@ -5388,7 +5397,7 @@
         <v>9</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N70" s="4" t="s">
         <v>89</v>
@@ -5396,34 +5405,34 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J71" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K71" s="6" t="s">
         <v>85</v>
@@ -5432,7 +5441,7 @@
         <v>9</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N71" s="4" t="s">
         <v>89</v>
@@ -5440,34 +5449,34 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I72" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J72" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K72" s="6" t="s">
         <v>85</v>
@@ -5476,7 +5485,7 @@
         <v>9</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N72" s="4" t="s">
         <v>89</v>
@@ -5484,31 +5493,31 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G73" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="H73" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="H73" s="1" t="s">
-        <v>398</v>
-      </c>
       <c r="I73" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>95</v>
@@ -5528,34 +5537,34 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K74" s="6" t="s">
         <v>85</v>
@@ -5572,34 +5581,34 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J75" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K75" s="6" t="s">
         <v>85</v>
@@ -5616,31 +5625,31 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I76" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J76" s="6" t="s">
         <v>9</v>
@@ -5660,31 +5669,31 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>9</v>
@@ -5704,31 +5713,31 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J78" s="6" t="s">
         <v>9</v>
@@ -5748,31 +5757,31 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J79" s="6" t="s">
         <v>9</v>
@@ -5792,34 +5801,34 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K80" s="6" t="s">
         <v>85</v>
@@ -5828,7 +5837,7 @@
         <v>9</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N80" s="4" t="s">
         <v>89</v>
@@ -5836,34 +5845,34 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K81" s="6" t="s">
         <v>85</v>
@@ -5872,7 +5881,7 @@
         <v>9</v>
       </c>
       <c r="M81" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N81" s="4" t="s">
         <v>89</v>
@@ -5880,34 +5889,34 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K82" s="6" t="s">
         <v>85</v>
@@ -5916,7 +5925,7 @@
         <v>9</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N82" s="4" t="s">
         <v>89</v>
@@ -5924,34 +5933,34 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K83" s="6" t="s">
         <v>85</v>
@@ -5960,7 +5969,7 @@
         <v>9</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N83" s="4" t="s">
         <v>89</v>
@@ -5968,34 +5977,34 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K84" s="6" t="s">
         <v>85</v>
@@ -6004,7 +6013,7 @@
         <v>9</v>
       </c>
       <c r="M84" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>89</v>
@@ -6012,34 +6021,34 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I85" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K85" s="6" t="s">
         <v>85</v>
@@ -6048,7 +6057,7 @@
         <v>9</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N85" s="4" t="s">
         <v>89</v>
@@ -6056,43 +6065,43 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J86" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L86" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>89</v>
@@ -6100,43 +6109,43 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I87" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J87" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L87" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>89</v>
@@ -6144,37 +6153,37 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G88" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="H88" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="H88" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="I88" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>95</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L88" s="6" t="s">
         <v>9</v>
@@ -6188,43 +6197,43 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I89" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J89" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L89" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M89" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N89" s="4" t="s">
         <v>89</v>
@@ -6232,31 +6241,31 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>95</v>
@@ -6276,34 +6285,34 @@
     </row>
     <row r="91" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="B91" s="19" t="s">
         <v>433</v>
-      </c>
-      <c r="B91" s="19" t="s">
-        <v>434</v>
       </c>
       <c r="C91" s="20" t="s">
         <v>26</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E91" s="19" t="s">
         <v>50</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G91" s="18" t="s">
+        <v>437</v>
+      </c>
+      <c r="H91" s="18" t="s">
+        <v>436</v>
+      </c>
+      <c r="I91" s="19" t="s">
+        <v>425</v>
+      </c>
+      <c r="J91" s="21" t="s">
         <v>438</v>
-      </c>
-      <c r="H91" s="18" t="s">
-        <v>437</v>
-      </c>
-      <c r="I91" s="19" t="s">
-        <v>426</v>
-      </c>
-      <c r="J91" s="20" t="s">
-        <v>221</v>
       </c>
       <c r="K91" s="20" t="s">
         <v>94</v>
@@ -7107,49 +7116,49 @@
     <row r="73" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" t="s">
+        <v>226</v>
+      </c>
+      <c r="E73" t="s">
         <v>227</v>
       </c>
-      <c r="E73" t="s">
-        <v>228</v>
-      </c>
       <c r="G73" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" t="s">
+        <v>228</v>
+      </c>
+      <c r="E74" t="s">
         <v>229</v>
       </c>
-      <c r="E74" t="s">
-        <v>230</v>
-      </c>
       <c r="G74" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" t="s">
+        <v>230</v>
+      </c>
+      <c r="E75" t="s">
         <v>231</v>
       </c>
-      <c r="E75" t="s">
-        <v>232</v>
-      </c>
       <c r="G75" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" t="s">
+        <v>232</v>
+      </c>
+      <c r="E76" t="s">
         <v>233</v>
       </c>
-      <c r="E76" t="s">
-        <v>234</v>
-      </c>
       <c r="G76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SNUxIM distribution modify OVC to allow for caregiver
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1E6A2871-6E84-9249-B036-D34EB012F8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FA8AB1E2-D8C6-C749-8D49-B5C357D8A5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35280" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Unused FY19 targets" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'19Tto20TMap'!$A$1:$N$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'19Tto20TMap'!$A$1:$N$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -962,12 +962,6 @@
     <t>PMTCT PostANC/Age/Sex/Result</t>
   </si>
   <si>
-    <t>Age/Sex/ProgramStatus</t>
-  </si>
-  <si>
-    <t>QG5SE83IVmL</t>
-  </si>
-  <si>
     <t>GEND_GBV.PE.T</t>
   </si>
   <si>
@@ -1356,6 +1350,12 @@
   </si>
   <si>
     <t>&lt;01-18+ (OVC &amp; Caregivers)</t>
+  </si>
+  <si>
+    <t>QG5SE83IVmL;AtKTQ515PWr</t>
+  </si>
+  <si>
+    <t>Age/Sex/ProgramStatus;Age/Sex/ProgramStatusCaregiver</t>
   </si>
 </sst>
 </file>
@@ -2296,12 +2296,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="J91" sqref="J91"/>
+      <selection pane="topRight" activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2313,7 +2314,7 @@
     <col min="5" max="5" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2367,12 +2368,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
@@ -2393,7 +2394,7 @@
         <v>282</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>
@@ -2411,12 +2412,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -2437,7 +2438,7 @@
         <v>282</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>9</v>
@@ -2455,12 +2456,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>287</v>
@@ -2481,10 +2482,10 @@
         <v>269</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>85</v>
@@ -2499,12 +2500,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>287</v>
@@ -2525,10 +2526,10 @@
         <v>269</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>85</v>
@@ -2543,18 +2544,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>50</v>
@@ -2563,13 +2564,13 @@
         <v>241</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>95</v>
@@ -2587,12 +2588,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>287</v>
@@ -2613,10 +2614,10 @@
         <v>268</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>85</v>
@@ -2631,12 +2632,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>287</v>
@@ -2657,10 +2658,10 @@
         <v>268</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>85</v>
@@ -2675,18 +2676,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>50</v>
@@ -2695,13 +2696,13 @@
         <v>241</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>95</v>
@@ -2719,12 +2720,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>17</v>
@@ -2745,7 +2746,7 @@
         <v>264</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>84</v>
@@ -2763,12 +2764,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>19</v>
@@ -2789,7 +2790,7 @@
         <v>267</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>86</v>
@@ -2807,12 +2808,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>19</v>
@@ -2833,7 +2834,7 @@
         <v>267</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>86</v>
@@ -2851,18 +2852,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>50</v>
@@ -2871,13 +2872,13 @@
         <v>241</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>95</v>
@@ -2895,12 +2896,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>19</v>
@@ -2921,7 +2922,7 @@
         <v>270</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>86</v>
@@ -2939,12 +2940,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>19</v>
@@ -2965,7 +2966,7 @@
         <v>270</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>86</v>
@@ -2983,18 +2984,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>50</v>
@@ -3003,13 +3004,13 @@
         <v>241</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>95</v>
@@ -3027,12 +3028,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
@@ -3053,7 +3054,7 @@
         <v>274</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>87</v>
@@ -3071,12 +3072,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>19</v>
@@ -3097,7 +3098,7 @@
         <v>274</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>87</v>
@@ -3115,12 +3116,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>19</v>
@@ -3141,7 +3142,7 @@
         <v>283</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>86</v>
@@ -3159,12 +3160,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>19</v>
@@ -3185,7 +3186,7 @@
         <v>283</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>86</v>
@@ -3203,18 +3204,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>50</v>
@@ -3223,13 +3224,13 @@
         <v>241</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>95</v>
@@ -3247,12 +3248,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>19</v>
@@ -3273,7 +3274,7 @@
         <v>276</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>86</v>
@@ -3291,12 +3292,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>19</v>
@@ -3317,7 +3318,7 @@
         <v>276</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>86</v>
@@ -3335,18 +3336,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>50</v>
@@ -3355,13 +3356,13 @@
         <v>241</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>95</v>
@@ -3379,12 +3380,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>19</v>
@@ -3405,7 +3406,7 @@
         <v>277</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>86</v>
@@ -3423,12 +3424,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>19</v>
@@ -3449,7 +3450,7 @@
         <v>277</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>86</v>
@@ -3467,18 +3468,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>50</v>
@@ -3487,13 +3488,13 @@
         <v>241</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>95</v>
@@ -3511,12 +3512,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>19</v>
@@ -3537,7 +3538,7 @@
         <v>278</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>87</v>
@@ -3555,12 +3556,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>19</v>
@@ -3581,7 +3582,7 @@
         <v>278</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>87</v>
@@ -3599,12 +3600,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>19</v>
@@ -3625,10 +3626,10 @@
         <v>305</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>94</v>
@@ -3643,12 +3644,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>19</v>
@@ -3669,10 +3670,10 @@
         <v>305</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>94</v>
@@ -3687,18 +3688,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>50</v>
@@ -3707,13 +3708,13 @@
         <v>241</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>95</v>
@@ -3731,12 +3732,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>19</v>
@@ -3757,7 +3758,7 @@
         <v>280</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>86</v>
@@ -3775,12 +3776,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>19</v>
@@ -3801,7 +3802,7 @@
         <v>280</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>86</v>
@@ -3819,18 +3820,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>50</v>
@@ -3839,13 +3840,13 @@
         <v>241</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>95</v>
@@ -3863,12 +3864,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>19</v>
@@ -3889,7 +3890,7 @@
         <v>281</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>86</v>
@@ -3907,12 +3908,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>19</v>
@@ -3933,7 +3934,7 @@
         <v>281</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>86</v>
@@ -3951,18 +3952,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>50</v>
@@ -3971,13 +3972,13 @@
         <v>241</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>95</v>
@@ -3995,12 +3996,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>19</v>
@@ -4021,7 +4022,7 @@
         <v>273</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J39" s="6" t="s">
         <v>9</v>
@@ -4039,12 +4040,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>19</v>
@@ -4065,7 +4066,7 @@
         <v>273</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>9</v>
@@ -4083,12 +4084,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
@@ -4109,7 +4110,7 @@
         <v>271</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>9</v>
@@ -4127,18 +4128,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>50</v>
@@ -4153,7 +4154,7 @@
         <v>272</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>9</v>
@@ -4171,12 +4172,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>21</v>
@@ -4197,7 +4198,7 @@
         <v>279</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>9</v>
@@ -4215,12 +4216,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>23</v>
@@ -4241,7 +4242,7 @@
         <v>271</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>9</v>
@@ -4259,12 +4260,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>25</v>
@@ -4285,7 +4286,7 @@
         <v>275</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>9</v>
@@ -4305,10 +4306,10 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>26</v>
@@ -4323,16 +4324,16 @@
         <v>241</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>307</v>
+        <v>438</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>308</v>
+        <v>437</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J46" s="21" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K46" s="6" t="s">
         <v>85</v>
@@ -4349,10 +4350,10 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>26</v>
@@ -4367,16 +4368,16 @@
         <v>241</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>307</v>
+        <v>438</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>308</v>
+        <v>437</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J47" s="21" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K47" s="6" t="s">
         <v>85</v>
@@ -4393,10 +4394,10 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>26</v>
@@ -4411,16 +4412,16 @@
         <v>241</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="K48" s="14" t="s">
         <v>85</v>
@@ -4435,12 +4436,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>27</v>
@@ -4461,10 +4462,10 @@
         <v>292</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K49" s="6" t="s">
         <v>94</v>
@@ -4479,12 +4480,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>27</v>
@@ -4505,10 +4506,10 @@
         <v>292</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K50" s="6" t="s">
         <v>94</v>
@@ -4523,12 +4524,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>28</v>
@@ -4549,7 +4550,7 @@
         <v>263</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>92</v>
@@ -4567,12 +4568,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>28</v>
@@ -4593,7 +4594,7 @@
         <v>263</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>93</v>
@@ -4611,12 +4612,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>30</v>
@@ -4637,10 +4638,10 @@
         <v>264</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>94</v>
@@ -4655,12 +4656,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>30</v>
@@ -4681,10 +4682,10 @@
         <v>266</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K54" s="6" t="s">
         <v>94</v>
@@ -4699,12 +4700,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>30</v>
@@ -4725,10 +4726,10 @@
         <v>266</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>94</v>
@@ -4743,12 +4744,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>30</v>
@@ -4769,10 +4770,10 @@
         <v>266</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K56" s="6" t="s">
         <v>94</v>
@@ -4787,33 +4788,33 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>395</v>
-      </c>
       <c r="I57" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>95</v>
@@ -4831,12 +4832,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>33</v>
@@ -4857,7 +4858,7 @@
         <v>264</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>84</v>
@@ -4875,12 +4876,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>34</v>
@@ -4901,7 +4902,7 @@
         <v>264</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>95</v>
@@ -4919,12 +4920,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>34</v>
@@ -4945,7 +4946,7 @@
         <v>271</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J60" s="6" t="s">
         <v>9</v>
@@ -4963,12 +4964,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>35</v>
@@ -4989,7 +4990,7 @@
         <v>264</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>95</v>
@@ -5007,12 +5008,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>35</v>
@@ -5033,7 +5034,7 @@
         <v>271</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>9</v>
@@ -5051,12 +5052,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>36</v>
@@ -5077,10 +5078,10 @@
         <v>292</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J63" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K63" s="6" t="s">
         <v>85</v>
@@ -5095,12 +5096,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>36</v>
@@ -5121,10 +5122,10 @@
         <v>292</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K64" s="6" t="s">
         <v>85</v>
@@ -5139,12 +5140,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>37</v>
@@ -5165,7 +5166,7 @@
         <v>292</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>286</v>
@@ -5183,12 +5184,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>37</v>
@@ -5209,7 +5210,7 @@
         <v>292</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>286</v>
@@ -5227,12 +5228,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>37</v>
@@ -5253,7 +5254,7 @@
         <v>292</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>286</v>
@@ -5271,12 +5272,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>37</v>
@@ -5297,7 +5298,7 @@
         <v>292</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>286</v>
@@ -5315,12 +5316,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>38</v>
@@ -5341,10 +5342,10 @@
         <v>264</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K69" s="6" t="s">
         <v>85</v>
@@ -5359,12 +5360,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>38</v>
@@ -5385,10 +5386,10 @@
         <v>266</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K70" s="6" t="s">
         <v>85</v>
@@ -5403,12 +5404,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>38</v>
@@ -5429,10 +5430,10 @@
         <v>266</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J71" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K71" s="6" t="s">
         <v>85</v>
@@ -5447,12 +5448,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>38</v>
@@ -5473,10 +5474,10 @@
         <v>266</v>
       </c>
       <c r="I72" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J72" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K72" s="6" t="s">
         <v>85</v>
@@ -5491,18 +5492,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>50</v>
@@ -5511,13 +5512,13 @@
         <v>241</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>95</v>
@@ -5535,12 +5536,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>39</v>
@@ -5561,10 +5562,10 @@
         <v>265</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K74" s="6" t="s">
         <v>85</v>
@@ -5579,12 +5580,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>40</v>
@@ -5605,10 +5606,10 @@
         <v>265</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J75" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K75" s="6" t="s">
         <v>85</v>
@@ -5623,12 +5624,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>40</v>
@@ -5649,7 +5650,7 @@
         <v>272</v>
       </c>
       <c r="I76" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J76" s="6" t="s">
         <v>9</v>
@@ -5667,12 +5668,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>39</v>
@@ -5693,7 +5694,7 @@
         <v>272</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>9</v>
@@ -5711,12 +5712,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>42</v>
@@ -5737,7 +5738,7 @@
         <v>272</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J78" s="6" t="s">
         <v>9</v>
@@ -5755,12 +5756,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>42</v>
@@ -5781,7 +5782,7 @@
         <v>272</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J79" s="6" t="s">
         <v>9</v>
@@ -5799,12 +5800,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>42</v>
@@ -5825,10 +5826,10 @@
         <v>294</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K80" s="6" t="s">
         <v>85</v>
@@ -5843,12 +5844,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>42</v>
@@ -5869,10 +5870,10 @@
         <v>294</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K81" s="6" t="s">
         <v>85</v>
@@ -5887,12 +5888,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>44</v>
@@ -5913,7 +5914,7 @@
         <v>298</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>286</v>
@@ -5931,12 +5932,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>44</v>
@@ -5957,7 +5958,7 @@
         <v>298</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J83" s="4" t="s">
         <v>286</v>
@@ -5975,12 +5976,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>44</v>
@@ -6001,7 +6002,7 @@
         <v>298</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>286</v>
@@ -6019,12 +6020,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>44</v>
@@ -6045,7 +6046,7 @@
         <v>298</v>
       </c>
       <c r="I85" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J85" s="4" t="s">
         <v>286</v>
@@ -6063,12 +6064,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>46</v>
@@ -6089,10 +6090,10 @@
         <v>265</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J86" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K86" s="6" t="s">
         <v>235</v>
@@ -6107,12 +6108,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>46</v>
@@ -6133,10 +6134,10 @@
         <v>265</v>
       </c>
       <c r="I87" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J87" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K87" s="6" t="s">
         <v>235</v>
@@ -6151,18 +6152,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>50</v>
@@ -6171,13 +6172,13 @@
         <v>241</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I88" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>95</v>
@@ -6195,12 +6196,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>46</v>
@@ -6221,10 +6222,10 @@
         <v>265</v>
       </c>
       <c r="I89" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J89" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K89" s="6" t="s">
         <v>235</v>
@@ -6239,12 +6240,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>6</v>
@@ -6265,7 +6266,7 @@
         <v>265</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>95</v>
@@ -6285,10 +6286,10 @@
     </row>
     <row r="91" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C91" s="20" t="s">
         <v>26</v>
@@ -6303,16 +6304,16 @@
         <v>241</v>
       </c>
       <c r="G91" s="18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H91" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="I91" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="J91" s="21" t="s">
         <v>436</v>
-      </c>
-      <c r="I91" s="19" t="s">
-        <v>425</v>
-      </c>
-      <c r="J91" s="21" t="s">
-        <v>438</v>
       </c>
       <c r="K91" s="20" t="s">
         <v>94</v>
@@ -6328,6 +6329,16 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N91" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="OVC_SERV.Active.T"/>
+        <filter val="OVC_SERV.DREAMS.T"/>
+        <filter val="OVC_SERV.Grad.T"/>
+        <filter val="OVC_SERV.Prev.T"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N90">
     <sortCondition ref="A2:A90"/>
   </sortState>
@@ -7171,7 +7182,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Psn ux im updates (#42)
* SNUxIM distribution modify OVC to allow for caregiver

* Update SnuXimMapAnalysis.R

* Update DESCRIPTION
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/22Tto23TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1E6A2871-6E84-9249-B036-D34EB012F8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FA8AB1E2-D8C6-C749-8D49-B5C357D8A5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35280" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Unused FY19 targets" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'19Tto20TMap'!$A$1:$N$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'19Tto20TMap'!$A$1:$N$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -962,12 +962,6 @@
     <t>PMTCT PostANC/Age/Sex/Result</t>
   </si>
   <si>
-    <t>Age/Sex/ProgramStatus</t>
-  </si>
-  <si>
-    <t>QG5SE83IVmL</t>
-  </si>
-  <si>
     <t>GEND_GBV.PE.T</t>
   </si>
   <si>
@@ -1356,6 +1350,12 @@
   </si>
   <si>
     <t>&lt;01-18+ (OVC &amp; Caregivers)</t>
+  </si>
+  <si>
+    <t>QG5SE83IVmL;AtKTQ515PWr</t>
+  </si>
+  <si>
+    <t>Age/Sex/ProgramStatus;Age/Sex/ProgramStatusCaregiver</t>
   </si>
 </sst>
 </file>
@@ -2296,12 +2296,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A44" sqref="A44"/>
-      <selection pane="topRight" activeCell="J91" sqref="J91"/>
+      <selection pane="topRight" activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2313,7 +2314,7 @@
     <col min="5" max="5" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2367,12 +2368,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
@@ -2393,7 +2394,7 @@
         <v>282</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>
@@ -2411,12 +2412,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -2437,7 +2438,7 @@
         <v>282</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>9</v>
@@ -2455,12 +2456,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>287</v>
@@ -2481,10 +2482,10 @@
         <v>269</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>85</v>
@@ -2499,12 +2500,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>287</v>
@@ -2525,10 +2526,10 @@
         <v>269</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>85</v>
@@ -2543,18 +2544,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>50</v>
@@ -2563,13 +2564,13 @@
         <v>241</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>95</v>
@@ -2587,12 +2588,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>287</v>
@@ -2613,10 +2614,10 @@
         <v>268</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>85</v>
@@ -2631,12 +2632,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>287</v>
@@ -2657,10 +2658,10 @@
         <v>268</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>85</v>
@@ -2675,18 +2676,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>50</v>
@@ -2695,13 +2696,13 @@
         <v>241</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>95</v>
@@ -2719,12 +2720,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>17</v>
@@ -2745,7 +2746,7 @@
         <v>264</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>84</v>
@@ -2763,12 +2764,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>19</v>
@@ -2789,7 +2790,7 @@
         <v>267</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>86</v>
@@ -2807,12 +2808,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>19</v>
@@ -2833,7 +2834,7 @@
         <v>267</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>86</v>
@@ -2851,18 +2852,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>50</v>
@@ -2871,13 +2872,13 @@
         <v>241</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>95</v>
@@ -2895,12 +2896,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>19</v>
@@ -2921,7 +2922,7 @@
         <v>270</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>86</v>
@@ -2939,12 +2940,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>19</v>
@@ -2965,7 +2966,7 @@
         <v>270</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>86</v>
@@ -2983,18 +2984,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>50</v>
@@ -3003,13 +3004,13 @@
         <v>241</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>95</v>
@@ -3027,12 +3028,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
@@ -3053,7 +3054,7 @@
         <v>274</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>87</v>
@@ -3071,12 +3072,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>19</v>
@@ -3097,7 +3098,7 @@
         <v>274</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>87</v>
@@ -3115,12 +3116,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>19</v>
@@ -3141,7 +3142,7 @@
         <v>283</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>86</v>
@@ -3159,12 +3160,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>19</v>
@@ -3185,7 +3186,7 @@
         <v>283</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>86</v>
@@ -3203,18 +3204,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>50</v>
@@ -3223,13 +3224,13 @@
         <v>241</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>95</v>
@@ -3247,12 +3248,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>19</v>
@@ -3273,7 +3274,7 @@
         <v>276</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>86</v>
@@ -3291,12 +3292,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>19</v>
@@ -3317,7 +3318,7 @@
         <v>276</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>86</v>
@@ -3335,18 +3336,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>50</v>
@@ -3355,13 +3356,13 @@
         <v>241</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>95</v>
@@ -3379,12 +3380,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>19</v>
@@ -3405,7 +3406,7 @@
         <v>277</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>86</v>
@@ -3423,12 +3424,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>19</v>
@@ -3449,7 +3450,7 @@
         <v>277</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>86</v>
@@ -3467,18 +3468,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>50</v>
@@ -3487,13 +3488,13 @@
         <v>241</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>95</v>
@@ -3511,12 +3512,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>19</v>
@@ -3537,7 +3538,7 @@
         <v>278</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>87</v>
@@ -3555,12 +3556,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>19</v>
@@ -3581,7 +3582,7 @@
         <v>278</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>87</v>
@@ -3599,12 +3600,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>19</v>
@@ -3625,10 +3626,10 @@
         <v>305</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>94</v>
@@ -3643,12 +3644,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>19</v>
@@ -3669,10 +3670,10 @@
         <v>305</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>94</v>
@@ -3687,18 +3688,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>50</v>
@@ -3707,13 +3708,13 @@
         <v>241</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>95</v>
@@ -3731,12 +3732,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>19</v>
@@ -3757,7 +3758,7 @@
         <v>280</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>86</v>
@@ -3775,12 +3776,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>19</v>
@@ -3801,7 +3802,7 @@
         <v>280</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>86</v>
@@ -3819,18 +3820,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>50</v>
@@ -3839,13 +3840,13 @@
         <v>241</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>95</v>
@@ -3863,12 +3864,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>19</v>
@@ -3889,7 +3890,7 @@
         <v>281</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>86</v>
@@ -3907,12 +3908,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>19</v>
@@ -3933,7 +3934,7 @@
         <v>281</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>86</v>
@@ -3951,18 +3952,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>50</v>
@@ -3971,13 +3972,13 @@
         <v>241</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>95</v>
@@ -3995,12 +3996,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>19</v>
@@ -4021,7 +4022,7 @@
         <v>273</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J39" s="6" t="s">
         <v>9</v>
@@ -4039,12 +4040,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>19</v>
@@ -4065,7 +4066,7 @@
         <v>273</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>9</v>
@@ -4083,12 +4084,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
@@ -4109,7 +4110,7 @@
         <v>271</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>9</v>
@@ -4127,18 +4128,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>50</v>
@@ -4153,7 +4154,7 @@
         <v>272</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>9</v>
@@ -4171,12 +4172,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>21</v>
@@ -4197,7 +4198,7 @@
         <v>279</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>9</v>
@@ -4215,12 +4216,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>23</v>
@@ -4241,7 +4242,7 @@
         <v>271</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>9</v>
@@ -4259,12 +4260,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>25</v>
@@ -4285,7 +4286,7 @@
         <v>275</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>9</v>
@@ -4305,10 +4306,10 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>26</v>
@@ -4323,16 +4324,16 @@
         <v>241</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>307</v>
+        <v>438</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>308</v>
+        <v>437</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J46" s="21" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K46" s="6" t="s">
         <v>85</v>
@@ -4349,10 +4350,10 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>26</v>
@@ -4367,16 +4368,16 @@
         <v>241</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>307</v>
+        <v>438</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>308</v>
+        <v>437</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J47" s="21" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K47" s="6" t="s">
         <v>85</v>
@@ -4393,10 +4394,10 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>26</v>
@@ -4411,16 +4412,16 @@
         <v>241</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="K48" s="14" t="s">
         <v>85</v>
@@ -4435,12 +4436,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>27</v>
@@ -4461,10 +4462,10 @@
         <v>292</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K49" s="6" t="s">
         <v>94</v>
@@ -4479,12 +4480,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>27</v>
@@ -4505,10 +4506,10 @@
         <v>292</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K50" s="6" t="s">
         <v>94</v>
@@ -4523,12 +4524,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>28</v>
@@ -4549,7 +4550,7 @@
         <v>263</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>92</v>
@@ -4567,12 +4568,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>28</v>
@@ -4593,7 +4594,7 @@
         <v>263</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>93</v>
@@ -4611,12 +4612,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>30</v>
@@ -4637,10 +4638,10 @@
         <v>264</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>94</v>
@@ -4655,12 +4656,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>30</v>
@@ -4681,10 +4682,10 @@
         <v>266</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K54" s="6" t="s">
         <v>94</v>
@@ -4699,12 +4700,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>30</v>
@@ -4725,10 +4726,10 @@
         <v>266</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>94</v>
@@ -4743,12 +4744,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>30</v>
@@ -4769,10 +4770,10 @@
         <v>266</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K56" s="6" t="s">
         <v>94</v>
@@ -4787,33 +4788,33 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>395</v>
-      </c>
       <c r="I57" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>95</v>
@@ -4831,12 +4832,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>33</v>
@@ -4857,7 +4858,7 @@
         <v>264</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>84</v>
@@ -4875,12 +4876,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>34</v>
@@ -4901,7 +4902,7 @@
         <v>264</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>95</v>
@@ -4919,12 +4920,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>34</v>
@@ -4945,7 +4946,7 @@
         <v>271</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J60" s="6" t="s">
         <v>9</v>
@@ -4963,12 +4964,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>35</v>
@@ -4989,7 +4990,7 @@
         <v>264</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>95</v>
@@ -5007,12 +5008,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>35</v>
@@ -5033,7 +5034,7 @@
         <v>271</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>9</v>
@@ -5051,12 +5052,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>36</v>
@@ -5077,10 +5078,10 @@
         <v>292</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J63" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K63" s="6" t="s">
         <v>85</v>
@@ -5095,12 +5096,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>36</v>
@@ -5121,10 +5122,10 @@
         <v>292</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K64" s="6" t="s">
         <v>85</v>
@@ -5139,12 +5140,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>37</v>
@@ -5165,7 +5166,7 @@
         <v>292</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>286</v>
@@ -5183,12 +5184,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>37</v>
@@ -5209,7 +5210,7 @@
         <v>292</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>286</v>
@@ -5227,12 +5228,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>37</v>
@@ -5253,7 +5254,7 @@
         <v>292</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>286</v>
@@ -5271,12 +5272,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>37</v>
@@ -5297,7 +5298,7 @@
         <v>292</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>286</v>
@@ -5315,12 +5316,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>38</v>
@@ -5341,10 +5342,10 @@
         <v>264</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K69" s="6" t="s">
         <v>85</v>
@@ -5359,12 +5360,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>38</v>
@@ -5385,10 +5386,10 @@
         <v>266</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K70" s="6" t="s">
         <v>85</v>
@@ -5403,12 +5404,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>38</v>
@@ -5429,10 +5430,10 @@
         <v>266</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J71" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K71" s="6" t="s">
         <v>85</v>
@@ -5447,12 +5448,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>38</v>
@@ -5473,10 +5474,10 @@
         <v>266</v>
       </c>
       <c r="I72" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J72" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K72" s="6" t="s">
         <v>85</v>
@@ -5491,18 +5492,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>50</v>
@@ -5511,13 +5512,13 @@
         <v>241</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>95</v>
@@ -5535,12 +5536,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>39</v>
@@ -5561,10 +5562,10 @@
         <v>265</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K74" s="6" t="s">
         <v>85</v>
@@ -5579,12 +5580,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>40</v>
@@ -5605,10 +5606,10 @@
         <v>265</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J75" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K75" s="6" t="s">
         <v>85</v>
@@ -5623,12 +5624,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>40</v>
@@ -5649,7 +5650,7 @@
         <v>272</v>
       </c>
       <c r="I76" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J76" s="6" t="s">
         <v>9</v>
@@ -5667,12 +5668,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>39</v>
@@ -5693,7 +5694,7 @@
         <v>272</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>9</v>
@@ -5711,12 +5712,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>42</v>
@@ -5737,7 +5738,7 @@
         <v>272</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J78" s="6" t="s">
         <v>9</v>
@@ -5755,12 +5756,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>42</v>
@@ -5781,7 +5782,7 @@
         <v>272</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J79" s="6" t="s">
         <v>9</v>
@@ -5799,12 +5800,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>42</v>
@@ -5825,10 +5826,10 @@
         <v>294</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J80" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K80" s="6" t="s">
         <v>85</v>
@@ -5843,12 +5844,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>42</v>
@@ -5869,10 +5870,10 @@
         <v>294</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K81" s="6" t="s">
         <v>85</v>
@@ -5887,12 +5888,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>44</v>
@@ -5913,7 +5914,7 @@
         <v>298</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>286</v>
@@ -5931,12 +5932,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>44</v>
@@ -5957,7 +5958,7 @@
         <v>298</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J83" s="4" t="s">
         <v>286</v>
@@ -5975,12 +5976,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>44</v>
@@ -6001,7 +6002,7 @@
         <v>298</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>286</v>
@@ -6019,12 +6020,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>44</v>
@@ -6045,7 +6046,7 @@
         <v>298</v>
       </c>
       <c r="I85" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J85" s="4" t="s">
         <v>286</v>
@@ -6063,12 +6064,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>46</v>
@@ -6089,10 +6090,10 @@
         <v>265</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J86" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K86" s="6" t="s">
         <v>235</v>
@@ -6107,12 +6108,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>46</v>
@@ -6133,10 +6134,10 @@
         <v>265</v>
       </c>
       <c r="I87" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J87" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K87" s="6" t="s">
         <v>235</v>
@@ -6151,18 +6152,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>50</v>
@@ -6171,13 +6172,13 @@
         <v>241</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I88" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>95</v>
@@ -6195,12 +6196,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>46</v>
@@ -6221,10 +6222,10 @@
         <v>265</v>
       </c>
       <c r="I89" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J89" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K89" s="6" t="s">
         <v>235</v>
@@ -6239,12 +6240,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>6</v>
@@ -6265,7 +6266,7 @@
         <v>265</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>95</v>
@@ -6285,10 +6286,10 @@
     </row>
     <row r="91" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C91" s="20" t="s">
         <v>26</v>
@@ -6303,16 +6304,16 @@
         <v>241</v>
       </c>
       <c r="G91" s="18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H91" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="I91" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="J91" s="21" t="s">
         <v>436</v>
-      </c>
-      <c r="I91" s="19" t="s">
-        <v>425</v>
-      </c>
-      <c r="J91" s="21" t="s">
-        <v>438</v>
       </c>
       <c r="K91" s="20" t="s">
         <v>94</v>
@@ -6328,6 +6329,16 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N91" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="OVC_SERV.Active.T"/>
+        <filter val="OVC_SERV.DREAMS.T"/>
+        <filter val="OVC_SERV.Grad.T"/>
+        <filter val="OVC_SERV.Prev.T"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N90">
     <sortCondition ref="A2:A90"/>
   </sortState>
@@ -7171,7 +7182,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>